<commit_message>
archivos para ejercicios Excel
</commit_message>
<xml_diff>
--- a/AGE(OPE2017)/EJERCICIOS/EXCEL 2010/00 archivos/10 - FUNCIONES MATEMÁTICAS/excel_fun_mat_06.xlsx
+++ b/AGE(OPE2017)/EJERCICIOS/EXCEL 2010/00 archivos/10 - FUNCIONES MATEMÁTICAS/excel_fun_mat_06.xlsx
@@ -7,11 +7,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="EJERCICIO 1" sheetId="1" r:id="rId1"/>
+    <sheet name="EJERCICIO 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Radianes">Hoja2!$B$2:$B$14</definedName>
+    <definedName name="Radianes">'EJERCICIO 2'!$B$2:$B$14</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -72,8 +72,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -141,9 +141,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -518,7 +518,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -806,7 +806,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C37" sqref="C37:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -837,274 +837,118 @@
       <c r="A2">
         <v>30</v>
       </c>
-      <c r="B2" s="2">
-        <f t="shared" ref="B2:B14" si="0">RADIANS(A2)</f>
-        <v>0.52359877559829882</v>
-      </c>
-      <c r="C2" s="6">
-        <f t="shared" ref="C2:C14" si="1">4*SIN(Radianes)^2</f>
-        <v>0.99999999999999978</v>
-      </c>
-      <c r="D2" s="7">
-        <f t="shared" ref="D2:D14" si="2">COS(Radianes)/2</f>
-        <v>0.43301270189221935</v>
-      </c>
-      <c r="E2" s="8">
-        <f t="shared" ref="E2:E14" si="3">TAN(Radianes)</f>
-        <v>0.57735026918962573</v>
-      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
         <v>35</v>
       </c>
-      <c r="B3" s="2">
-        <f t="shared" si="0"/>
-        <v>0.6108652381980153</v>
-      </c>
-      <c r="C3" s="6">
-        <f t="shared" si="1"/>
-        <v>1.3159597133486622</v>
-      </c>
-      <c r="D3" s="7">
-        <f t="shared" si="2"/>
-        <v>0.4095760221444959</v>
-      </c>
-      <c r="E3" s="8">
-        <f t="shared" si="3"/>
-        <v>0.70020753820970971</v>
-      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
         <v>40</v>
       </c>
-      <c r="B4" s="2">
-        <f t="shared" si="0"/>
-        <v>0.69813170079773179</v>
-      </c>
-      <c r="C4" s="6">
-        <f t="shared" si="1"/>
-        <v>1.6527036446661389</v>
-      </c>
-      <c r="D4" s="7">
-        <f t="shared" si="2"/>
-        <v>0.38302222155948901</v>
-      </c>
-      <c r="E4" s="8">
-        <f t="shared" si="3"/>
-        <v>0.83909963117727993</v>
-      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
         <v>45</v>
       </c>
-      <c r="B5" s="2">
-        <f t="shared" si="0"/>
-        <v>0.78539816339744828</v>
-      </c>
-      <c r="C5" s="6">
-        <f t="shared" si="1"/>
-        <v>1.9999999999999996</v>
-      </c>
-      <c r="D5" s="7">
-        <f t="shared" si="2"/>
-        <v>0.35355339059327379</v>
-      </c>
-      <c r="E5" s="8">
-        <f t="shared" si="3"/>
-        <v>0.99999999999999989</v>
-      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
         <v>50</v>
       </c>
-      <c r="B6" s="2">
-        <f t="shared" si="0"/>
-        <v>0.87266462599716477</v>
-      </c>
-      <c r="C6" s="6">
-        <f t="shared" si="1"/>
-        <v>2.3472963553338606</v>
-      </c>
-      <c r="D6" s="7">
-        <f t="shared" si="2"/>
-        <v>0.32139380484326968</v>
-      </c>
-      <c r="E6" s="8">
-        <f t="shared" si="3"/>
-        <v>1.19175359259421</v>
-      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
         <v>55</v>
       </c>
-      <c r="B7" s="2">
-        <f t="shared" si="0"/>
-        <v>0.95993108859688125</v>
-      </c>
-      <c r="C7" s="6">
-        <f t="shared" si="1"/>
-        <v>2.6840402866513373</v>
-      </c>
-      <c r="D7" s="7">
-        <f t="shared" si="2"/>
-        <v>0.28678821817552308</v>
-      </c>
-      <c r="E7" s="8">
-        <f t="shared" si="3"/>
-        <v>1.4281480067421144</v>
-      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
         <v>60</v>
       </c>
-      <c r="B8" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0471975511965976</v>
-      </c>
-      <c r="C8" s="6">
-        <f t="shared" si="1"/>
-        <v>2.9999999999999996</v>
-      </c>
-      <c r="D8" s="7">
-        <f t="shared" si="2"/>
-        <v>0.25000000000000006</v>
-      </c>
-      <c r="E8" s="8">
-        <f t="shared" si="3"/>
-        <v>1.7320508075688767</v>
-      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
         <v>65</v>
       </c>
-      <c r="B9" s="2">
-        <f t="shared" si="0"/>
-        <v>1.1344640137963142</v>
-      </c>
-      <c r="C9" s="6">
-        <f t="shared" si="1"/>
-        <v>3.2855752193730785</v>
-      </c>
-      <c r="D9" s="7">
-        <f t="shared" si="2"/>
-        <v>0.21130913087034972</v>
-      </c>
-      <c r="E9" s="8">
-        <f t="shared" si="3"/>
-        <v>2.1445069205095586</v>
-      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
         <v>70</v>
       </c>
-      <c r="B10" s="2">
-        <f t="shared" si="0"/>
-        <v>1.2217304763960306</v>
-      </c>
-      <c r="C10" s="6">
-        <f t="shared" si="1"/>
-        <v>3.5320888862379554</v>
-      </c>
-      <c r="D10" s="7">
-        <f t="shared" si="2"/>
-        <v>0.17101007166283441</v>
-      </c>
-      <c r="E10" s="8">
-        <f t="shared" si="3"/>
-        <v>2.7474774194546216</v>
-      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
         <v>75</v>
       </c>
-      <c r="B11" s="2">
-        <f t="shared" si="0"/>
-        <v>1.3089969389957472</v>
-      </c>
-      <c r="C11" s="6">
-        <f t="shared" si="1"/>
-        <v>3.7320508075688776</v>
-      </c>
-      <c r="D11" s="7">
-        <f t="shared" si="2"/>
-        <v>0.12940952255126037</v>
-      </c>
-      <c r="E11" s="8">
-        <f t="shared" si="3"/>
-        <v>3.7320508075688776</v>
-      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
         <v>80</v>
       </c>
-      <c r="B12" s="2">
-        <f t="shared" si="0"/>
-        <v>1.3962634015954636</v>
-      </c>
-      <c r="C12" s="6">
-        <f t="shared" si="1"/>
-        <v>3.8793852415718164</v>
-      </c>
-      <c r="D12" s="7">
-        <f t="shared" si="2"/>
-        <v>8.6824088833465207E-2</v>
-      </c>
-      <c r="E12" s="8">
-        <f t="shared" si="3"/>
-        <v>5.6712818196177066</v>
-      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
         <v>85</v>
       </c>
-      <c r="B13" s="2">
-        <f t="shared" si="0"/>
-        <v>1.4835298641951802</v>
-      </c>
-      <c r="C13" s="6">
-        <f t="shared" si="1"/>
-        <v>3.9696155060244163</v>
-      </c>
-      <c r="D13" s="7">
-        <f t="shared" si="2"/>
-        <v>4.3577871373829069E-2</v>
-      </c>
-      <c r="E13" s="8">
-        <f t="shared" si="3"/>
-        <v>11.430052302761348</v>
-      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
         <v>90</v>
       </c>
-      <c r="B14" s="2">
-        <f t="shared" si="0"/>
-        <v>1.5707963267948966</v>
-      </c>
-      <c r="C14" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="D14" s="7">
-        <f t="shared" si="2"/>
-        <v>3.06287113727155E-17</v>
-      </c>
-      <c r="E14" s="9">
-        <f t="shared" si="3"/>
-        <v>1.6324552277619072E+16</v>
-      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>